<commit_message>
Revise GetJournal.py to GridTableGetter.py
</commit_message>
<xml_diff>
--- a/CSSCI期刊.xlsx
+++ b/CSSCI期刊.xlsx
@@ -754,8 +754,10 @@
           <t>11-4054/D</t>
         </is>
       </c>
-      <c r="E13" t="n">
-        <v>32</v>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -777,8 +779,10 @@
           <t>11-3171/D</t>
         </is>
       </c>
-      <c r="E14" t="n">
-        <v>1</v>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -800,8 +804,10 @@
           <t>11-2878/G4</t>
         </is>
       </c>
-      <c r="E15" t="n">
-        <v>1</v>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -824,7 +830,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>1</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17">

</xml_diff>